<commit_message>
linear regression + emotional classification prog
</commit_message>
<xml_diff>
--- a/dataset_summaries.xlsx
+++ b/dataset_summaries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_summaries" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="datasets_post_cleaning" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="thread_data" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="failed threads" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Author thresholds" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="122">
   <si>
     <t xml:space="preserve">rows</t>
   </si>
@@ -387,6 +388,9 @@
   </si>
   <si>
     <t xml:space="preserve">p_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% authors with 1 activity</t>
   </si>
 </sst>
 </file>
@@ -403,6 +407,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -424,17 +429,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -445,12 +453,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -479,7 +494,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -496,7 +511,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -517,6 +532,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,6 +553,14 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -559,7 +586,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.13"/>
@@ -567,13 +594,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,9 +842,9 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.51"/>
@@ -1098,7 +1125,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1117,7 +1144,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -1339,7 +1366,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1358,11 +1385,11 @@
       <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2402,7 +2429,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2417,13 +2444,13 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,7 +2553,7 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
         <v>109</v>
       </c>
@@ -2790,28 +2817,28 @@
       <c r="A21" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="10" t="n">
         <v>0.08477</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="10" t="n">
         <v>0.058087</v>
       </c>
-      <c r="D21" s="9" t="n">
+      <c r="D21" s="10" t="n">
         <v>-0.049397</v>
       </c>
-      <c r="E21" s="9" t="n">
+      <c r="E21" s="10" t="n">
         <v>-0.072327</v>
       </c>
-      <c r="F21" s="9" t="n">
+      <c r="F21" s="10" t="n">
         <v>0.077023</v>
       </c>
-      <c r="G21" s="9" t="n">
+      <c r="G21" s="10" t="n">
         <v>0.022992</v>
       </c>
-      <c r="H21" s="9" t="n">
+      <c r="H21" s="10" t="n">
         <v>0.102594</v>
       </c>
-      <c r="I21" s="9" t="n">
+      <c r="I21" s="10" t="n">
         <v>0.090682</v>
       </c>
       <c r="J21" s="2" t="n">
@@ -2825,28 +2852,28 @@
       <c r="A22" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="10" t="n">
         <v>0.309465</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="10" t="n">
         <v>0.328576</v>
       </c>
-      <c r="D22" s="9" t="n">
+      <c r="D22" s="10" t="n">
         <v>0.318912</v>
       </c>
-      <c r="E22" s="9" t="n">
+      <c r="E22" s="10" t="n">
         <v>0.337043</v>
       </c>
-      <c r="F22" s="9" t="n">
+      <c r="F22" s="10" t="n">
         <v>0.28568</v>
       </c>
-      <c r="G22" s="9" t="n">
+      <c r="G22" s="10" t="n">
         <v>0.310779</v>
       </c>
-      <c r="H22" s="9" t="n">
+      <c r="H22" s="10" t="n">
         <v>0.352886</v>
       </c>
-      <c r="I22" s="9" t="n">
+      <c r="I22" s="10" t="n">
         <v>0.342914</v>
       </c>
       <c r="J22" s="2" t="n">
@@ -3042,7 +3069,7 @@
       <c r="F29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -3075,10 +3102,10 @@
       <c r="E31" s="2" t="n">
         <v>0.115784</v>
       </c>
-      <c r="F31" s="11" t="n">
+      <c r="F31" s="12" t="n">
         <v>0.08721867</v>
       </c>
-      <c r="J31" s="12"/>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
@@ -3096,47 +3123,47 @@
       <c r="E32" s="2" t="n">
         <v>0.095883</v>
       </c>
-      <c r="F32" s="11" t="n">
+      <c r="F32" s="12" t="n">
         <v>1.771323E-098</v>
       </c>
-      <c r="J32" s="12"/>
+      <c r="J32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
-      <c r="C33" s="11"/>
-      <c r="J33" s="12"/>
+      <c r="A33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="J33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
-      <c r="C34" s="11"/>
-      <c r="J34" s="12"/>
+      <c r="A34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="J34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13"/>
-      <c r="C35" s="11"/>
-      <c r="J35" s="13"/>
+      <c r="A35" s="14"/>
+      <c r="C35" s="12"/>
+      <c r="J35" s="14"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13"/>
-      <c r="C36" s="11"/>
-      <c r="J36" s="13"/>
+      <c r="A36" s="14"/>
+      <c r="C36" s="12"/>
+      <c r="J36" s="14"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13"/>
-      <c r="C37" s="11"/>
-      <c r="J37" s="13"/>
+      <c r="A37" s="14"/>
+      <c r="C37" s="12"/>
+      <c r="J37" s="14"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
-      <c r="C38" s="11"/>
-      <c r="J38" s="12"/>
+      <c r="A38" s="13"/>
+      <c r="C38" s="12"/>
+      <c r="J38" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="12"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3154,10 +3181,77 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.01"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="16" t="n">
+        <v>43.314904528553</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="16" t="n">
+        <v>46.9018695878339</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="16" t="n">
+        <v>42.3210269865068</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="16" t="n">
+        <v>68.0453694527034</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>